<commit_message>
added more wording to readme, added label div and styled label div in sass
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>key</t>
   </si>
@@ -23,6 +23,12 @@
   </si>
   <si>
     <t>Sig goes here</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Label goes here</t>
   </si>
   <si>
     <t>headline</t>
@@ -211,7 +217,7 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -219,7 +225,7 @@
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -235,20 +241,28 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>